<commit_message>
batch run settings updated in conf.js file
</commit_message>
<xml_diff>
--- a/LearnProtractor/test_data/CURA Appointment Data.xlsx
+++ b/LearnProtractor/test_data/CURA Appointment Data.xlsx
@@ -1,44 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Cred" sheetId="1" r:id="rId1"/>
-    <sheet name="Data Sets" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Sets" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
-  <si>
-    <t>AppURL</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>https://katalon-demo-cura.herokuapp.com/</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>ThisIsNotAPassword</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>FacilityName</t>
   </si>
@@ -55,31 +31,31 @@
     <t>Tokyo</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Medicare</t>
+  </si>
+  <si>
+    <t>16/09/2020</t>
+  </si>
+  <si>
     <t>Hongkong</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Medicaid</t>
+  </si>
+  <si>
+    <t>17/09/2020</t>
+  </si>
+  <si>
     <t>Seoul</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Medicare</t>
-  </si>
-  <si>
-    <t>Medicaid</t>
-  </si>
-  <si>
     <t>None</t>
-  </si>
-  <si>
-    <t>16/09/2020</t>
-  </si>
-  <si>
-    <t>17/09/2020</t>
   </si>
   <si>
     <t>18/09/2020</t>
@@ -89,7 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,23 +74,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
@@ -164,31 +125,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,108 +420,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>9</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -576,13 +483,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>20</v>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>